<commit_message>
add 7 8 12 13
</commit_message>
<xml_diff>
--- a/src/test/input/used/RFM/RFM-19.xlsx
+++ b/src/test/input/used/RFM/RFM-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse_workspace\LC_GEN\src\test\input\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A538BD02-E250-4EE1-A168-54E0D7822AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CBA06F-69B8-472B-BD66-1112EE5FD23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="51">
   <si>
     <t>BG/LC</t>
   </si>
@@ -70,107 +70,134 @@
     <t>Is Array</t>
   </si>
   <si>
-    <t>RFM-9</t>
+    <t>RFM-19</t>
   </si>
   <si>
     <t>NEW</t>
   </si>
   <si>
-    <t>refinancing-deal</t>
-  </si>
-  <si>
-    <t>Approve, SendBack, Reject, Cancel</t>
+    <t>Modify Document Details</t>
+  </si>
+  <si>
+    <t>This API will modify Document Details for Refinancing, Forfaiting and Risk Participation</t>
+  </si>
+  <si>
+    <t>Unique Identifier of Document Details. Applicable and mandatory only when CUD is U or D</t>
+  </si>
+  <si>
+    <t>document-id</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>REQUEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-id  </t>
+  </si>
+  <si>
+    <t>d_seqid</t>
+  </si>
+  <si>
+    <t>PUT /receivable-finance/{receivable-finance-type}/{receivable-finance-reference}/document-details</t>
   </si>
   <si>
     <t>Number of Original provided</t>
   </si>
   <si>
+    <t xml:space="preserve">number-of-original </t>
+  </si>
+  <si>
     <t>number(1)</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>REQUEST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number-of-original                     </t>
-  </si>
-  <si>
-    <t>This API will create Document Details for Refinancing, Forfaiting and Risk Participation</t>
-  </si>
-  <si>
-    <t>Qualifying remarks if any. Mandatory, if user action is Cancel, SendBack, reject</t>
+    <t>d_number01</t>
   </si>
   <si>
     <t>Number of Copies provided</t>
   </si>
   <si>
-    <t xml:space="preserve">number-of-copies                       </t>
-  </si>
-  <si>
-    <t>Refinancing Deal Pos Type</t>
+    <t>number-of-copies</t>
   </si>
   <si>
     <t>Document required or Document Submitted</t>
   </si>
   <si>
-    <t>varchar(20)</t>
+    <t>document-required-or-document-submitted</t>
+  </si>
+  <si>
+    <t>varchar</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>document-required-or-document-submitted</t>
-  </si>
-  <si>
-    <t>Refinancing Deal Pos ID</t>
-  </si>
-  <si>
-    <t>Nostro Credit CCY</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nostro-credit-ccy </t>
-  </si>
-  <si>
-    <t>d_currcode</t>
+    <t>d_alpha20</t>
+  </si>
+  <si>
+    <t>Create, Update, Delete</t>
+  </si>
+  <si>
+    <t>cud-indicator</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color indexed="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d_cudindicator</t>
+    </r>
   </si>
   <si>
     <t>This field will contain POS_Type</t>
   </si>
   <si>
-    <t>number</t>
+    <t>receivable-finance-type</t>
   </si>
   <si>
     <t>RESPONSE</t>
   </si>
   <si>
-    <t xml:space="preserve">receivable-finance-type       </t>
-  </si>
-  <si>
-    <t>d_PosTyp</t>
-  </si>
-  <si>
-    <t>PUT /receivable-finance/{receivable-finance-type}/{receivable-finance-reference}/document-details</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>refinancing-deal</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modify Document Details</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color indexed="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d_PosTyp</t>
+    </r>
+  </si>
+  <si>
+    <t>This field will contain POS_ID</t>
+  </si>
+  <si>
+    <t>receivable-finance-reference</t>
+  </si>
+  <si>
+    <t>This field will contain DOC_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cud-indicator </t>
+  </si>
+  <si>
+    <t>document-details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -204,6 +231,33 @@
       <family val="3"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color indexed="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="細明體"/>
       <family val="3"/>
@@ -224,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -258,6 +312,51 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
@@ -277,13 +376,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -300,27 +432,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{298C4F74-1154-4566-A62D-259FBF56FF6E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -337,7 +497,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFA1BFCC"/>
       <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="FF467886"/>
       <rgbColor rgb="000000FF"/>
       <rgbColor rgb="00FFFF00"/>
       <rgbColor rgb="00FF00FF"/>
@@ -1645,17 +1805,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IV6"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.59765625" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.1328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.86328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.73046875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.46484375" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.46484375" style="1" customWidth="1"/>
@@ -1725,248 +1885,454 @@
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="D2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="8" t="b">
+      <c r="L2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="D3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="11" t="b">
+      <c r="N3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="D4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="11" t="b">
+      <c r="M4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="I5" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="J5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" s="11" t="b">
+      <c r="M5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="G8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="D9" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="D10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="G10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="I10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="11" t="b">
+      <c r="M10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="18" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape"/>
   <headerFooter>

</xml_diff>